<commit_message>
version 2 work with gpio
</commit_message>
<xml_diff>
--- a/Documents/Таблица микросхем, плат и кода к ним.xlsx
+++ b/Documents/Таблица микросхем, плат и кода к ним.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="156">
   <si>
     <t>Название микросхемы:</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t>AT45DB641E-SHN2B</t>
+  </si>
+  <si>
+    <t>есть отдельная, есть команды для версии 2.0</t>
   </si>
 </sst>
 </file>
@@ -908,10 +911,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -1328,28 +1331,39 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="M16" s="8"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">

</xml_diff>

<commit_message>
add the chess order
</commit_message>
<xml_diff>
--- a/Documents/Таблица микросхем, плат и кода к ним.xlsx
+++ b/Documents/Таблица микросхем, плат и кода к ним.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Легенда" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$B$1:$N$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$B$1:$M$90</definedName>
   </definedNames>
   <calcPr calcId="162913" refMode="R1C1"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="157">
   <si>
     <t>Название микросхемы:</t>
   </si>
@@ -115,9 +115,6 @@
     <t>АСБД.418126.289</t>
   </si>
   <si>
-    <t>Универсальная прошивка</t>
-  </si>
-  <si>
     <t>Корпус</t>
   </si>
   <si>
@@ -478,9 +475,6 @@
     <t>отлаживал прошивку 2.0 на нем</t>
   </si>
   <si>
-    <t>Прошивка Макса</t>
-  </si>
-  <si>
     <t xml:space="preserve">GS82564Z18GB-400I </t>
   </si>
   <si>
@@ -491,6 +485,15 @@
   </si>
   <si>
     <t>есть отдельная, есть команды для версии 2.0</t>
+  </si>
+  <si>
+    <t>белая плата для выставки</t>
+  </si>
+  <si>
+    <t>Отдельный проект</t>
+  </si>
+  <si>
+    <t>паралельный</t>
   </si>
 </sst>
 </file>
@@ -593,7 +596,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -603,9 +606,6 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -619,13 +619,19 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -909,15 +915,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N90"/>
+  <dimension ref="A1:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="M16" sqref="M16"/>
+      <selection pane="bottomLeft" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" style="3" customWidth="1"/>
@@ -927,20 +933,19 @@
     <col min="6" max="6" width="23.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="23.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="32" style="3" customWidth="1"/>
-    <col min="12" max="12" width="36.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="44" style="3" customWidth="1"/>
-    <col min="14" max="14" width="27.5703125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="3"/>
-    <col min="16" max="16" width="14.5703125" style="3" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="3"/>
-    <col min="18" max="18" width="46" style="3" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="9" width="20" style="3" customWidth="1"/>
+    <col min="10" max="10" width="32" style="3" customWidth="1"/>
+    <col min="11" max="11" width="36.5703125" style="9" customWidth="1"/>
+    <col min="12" max="12" width="44" style="3" customWidth="1"/>
+    <col min="13" max="13" width="27.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="14.5703125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.140625" style="3"/>
+    <col min="17" max="17" width="46" style="3" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -951,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -963,57 +968,53 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>30</v>
+        <v>140</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>141</v>
+        <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="M2" s="8"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1021,74 +1022,74 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="M3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="8"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="I5" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="L5" s="7"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="I6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="M6" s="8"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1096,103 +1097,97 @@
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="M8" s="8"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="I9" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="M10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1203,10 +1198,10 @@
         <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>22</v>
@@ -1214,15 +1209,9 @@
       <c r="G11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1230,152 +1219,156 @@
         <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="M12" s="8"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="8" t="s">
+      <c r="D13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="M13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
+      <c r="G14" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="M14" s="8"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="D15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="M15" s="8"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H15" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="G16" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H16" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="M17" s="8"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E17" s="5"/>
+      <c r="L17" s="7"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -1383,112 +1376,107 @@
         <v>11</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="M18" s="8"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="L18" s="7"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M19" s="8"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M20" s="8"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>21</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="8" t="s">
+      <c r="G21" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="M21" s="8"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="E22" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="F22" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="M22" s="8"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L22" s="7"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="F23" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G23" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="M23" s="8"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L23" s="7"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>24</v>
       </c>
@@ -1496,384 +1484,345 @@
         <v>14</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="F24" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="M24" s="8"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>25</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>26</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F26" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="G26" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>27</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F27" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="G27" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="8"/>
-      <c r="J27" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8" t="s">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="G28" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F28" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="J28" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>29</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E29" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G29" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="I29" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="H30" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="M30" s="8"/>
-      <c r="N30" s="8"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+        <v>85</v>
+      </c>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+    </row>
+    <row r="31" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
         <v>31</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" s="5" t="s">
+      <c r="G31" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H31" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K31" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="M32" s="8"/>
-      <c r="N32" s="8"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>33</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M33" s="8"/>
-      <c r="N33" s="8"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>34</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>24</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E34" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J34" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K34" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M34" s="8"/>
-      <c r="N34" s="8"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>35</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="F35" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G35" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M36" s="8"/>
-      <c r="N36" s="8"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>37</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="M37" s="8"/>
-      <c r="N37" s="8"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>38</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>22</v>
@@ -1882,65 +1831,56 @@
         <v>23</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M38" s="8"/>
-      <c r="N38" s="8"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F39" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M39" s="8"/>
-      <c r="N39" s="8"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>40</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="M40" s="8"/>
-      <c r="N40" s="8"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>41</v>
       </c>
@@ -1948,13 +1888,13 @@
         <v>18</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>20</v>
@@ -1962,13 +1902,10 @@
       <c r="G41" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K41" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M41" s="8"/>
-      <c r="N41" s="8"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>42</v>
       </c>
@@ -1976,7 +1913,7 @@
         <v>27</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>29</v>
@@ -1984,253 +1921,253 @@
       <c r="G42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M42" s="8"/>
-      <c r="N42" s="8"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>43</v>
       </c>
-      <c r="M43" s="8"/>
-      <c r="N43" s="8"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>59</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>69</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>70</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>72</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>73</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>78</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>79</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>82</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>83</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>85</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>86</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>88</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>89</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:N90">
+  <autoFilter ref="B1:M90">
     <sortState ref="B2:N90">
       <sortCondition ref="B1:B90"/>
     </sortState>
@@ -2252,23 +2189,23 @@
   <sheetData>
     <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="5"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="10"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit after new branch
</commit_message>
<xml_diff>
--- a/Documents/Таблица микросхем, плат и кода к ним.xlsx
+++ b/Documents/Таблица микросхем, плат и кода к ним.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="161">
   <si>
     <t>Название микросхемы:</t>
   </si>
@@ -496,10 +496,16 @@
     <t>паралельный</t>
   </si>
   <si>
-    <t>28.02 словил баг, что в шахматном порядке первые две записи повторяются. Получается, что нужно добавить задержку перед чтением. Но в начале необходимо ее реализвать в коде (микросекундную)</t>
-  </si>
-  <si>
     <t>перед повторной записью необходимо стирать сектор</t>
+  </si>
+  <si>
+    <t>ПО верхнего уровня (версия 0.1)</t>
+  </si>
+  <si>
+    <t>проблемы с таймингами на общей прошивке</t>
+  </si>
+  <si>
+    <t>надо по новой перепроверить ПО верхнего уровня</t>
   </si>
 </sst>
 </file>
@@ -602,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -635,6 +641,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
@@ -920,10 +929,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="J36" sqref="J36"/>
+      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1263,13 +1272,13 @@
         <v>39</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>154</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
@@ -1325,41 +1334,44 @@
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="L15" s="7"/>
+      <c r="M15" s="3" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="10" t="s">
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="4" t="s">
+      <c r="L16" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="M16" s="7" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1665,36 +1677,34 @@
       <c r="A31" s="7">
         <v>31</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G31" s="4" t="s">
+      <c r="G31" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="I31" s="4" t="s">
+      <c r="I31" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="J31" s="4"/>
-      <c r="K31" s="10" t="s">
+      <c r="K31" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4" t="s">
+      <c r="M31" s="7" t="s">
         <v>149</v>
       </c>
     </row>
@@ -1852,7 +1862,7 @@
       <c r="L38" s="7"/>
       <c r="M38" s="7"/>
       <c r="N38" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add prog high level and add CY7C1019
</commit_message>
<xml_diff>
--- a/Documents/Таблица микросхем, плат и кода к ним.xlsx
+++ b/Documents/Таблица микросхем, плат и кода к ним.xlsx
@@ -929,10 +929,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="N14" sqref="N14"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1342,36 +1342,36 @@
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="12" t="s">
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="L16" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="M16" s="4" t="s">
         <v>149</v>
       </c>
     </row>

</xml_diff>